<commit_message>
correcion de errores en mate (permutaciones_combianciones.py) y algoritmos debido a conflictos del programa
</commit_message>
<xml_diff>
--- a/algoritmos/reportes/Reporte_Clientes.xlsx
+++ b/algoritmos/reportes/Reporte_Clientes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,49 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Sofia Vicente</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="n">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Miguel Gutierrez</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Perrito</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>38</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>